<commit_message>
Updated factor record after new features was introduced
</commit_message>
<xml_diff>
--- a/factor_record.xlsx
+++ b/factor_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern 1\Desktop\intern_work\Stock-market-predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6942072B-43FD-4E69-B472-AB02AF508286}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED734BA-4985-4AC2-A679-8AF00B420D2B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Ev/EBIDTA</t>
   </si>
@@ -40,15 +40,9 @@
     <t>Asset Turnover(x)</t>
   </si>
   <si>
-    <t>Div/ Yeild</t>
-  </si>
-  <si>
     <t>FR_PBIDTM(%)</t>
   </si>
   <si>
-    <t>FR_PATM(%)</t>
-  </si>
-  <si>
     <t>M/Sales</t>
   </si>
   <si>
@@ -67,9 +61,6 @@
     <t>FR_PATM (%)</t>
   </si>
   <si>
-    <t>Div/Yield</t>
-  </si>
-  <si>
     <t>PATM (%)</t>
   </si>
   <si>
@@ -80,13 +71,28 @@
   </si>
   <si>
     <t>Cons PAT</t>
+  </si>
+  <si>
+    <t>ROE</t>
+  </si>
+  <si>
+    <t>FR_Dividend Pay Out Ratio(%)</t>
+  </si>
+  <si>
+    <t>PL_Operating Profit (Excl OI)</t>
+  </si>
+  <si>
+    <t>Free Float</t>
+  </si>
+  <si>
+    <t>PAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +226,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -563,9 +593,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -924,7 +966,7 @@
   <dimension ref="A1:M122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,8 +1019,8 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -994,7 +1036,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1005,54 +1047,54 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>8</v>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>17</v>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -1063,24 +1105,24 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated factor_record.xlsx for 4 years
</commit_message>
<xml_diff>
--- a/factor_record.xlsx
+++ b/factor_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern 1\Desktop\intern_work\Stock-market-predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A7312A-7161-4817-9E3C-C5C58181C322}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E9B862-0AE6-4EC7-A37A-BE235DE59C06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>Ev/EBIDTA</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Net Sales | Cons OCF | ROCE(%) |Cons PAT | FR_Dividend Pay Out Ratio(%)</t>
+  </si>
+  <si>
+    <t>PBIDTM(%)</t>
   </si>
 </sst>
 </file>
@@ -258,7 +261,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,6 +450,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,7 +620,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -627,11 +636,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -990,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1047,6 +1061,9 @@
       <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1058,6 +1075,9 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1069,6 +1089,9 @@
       <c r="D4" t="s">
         <v>3</v>
       </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1080,6 +1103,9 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -1091,6 +1117,14 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1105,6 +1139,9 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -1116,6 +1153,9 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1127,6 +1167,9 @@
       <c r="D11" t="s">
         <v>3</v>
       </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1138,6 +1181,9 @@
       <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="E12" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1147,6 +1193,9 @@
         <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1163,65 +1212,77 @@
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1495,9 +1556,10 @@
       <c r="A122" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated till 2013 with sorted as correlation
</commit_message>
<xml_diff>
--- a/factor_record.xlsx
+++ b/factor_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern 1\Desktop\intern_work\Stock-market-predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1803F0-AFE7-4EEB-8CC0-F95CC40D4CB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA17389D-660A-457D-B88E-2122ECC6F7AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +259,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="36">
@@ -620,7 +626,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -646,6 +652,18 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1002,287 +1020,426 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M122"/>
+  <dimension ref="A1:Q122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>2010</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2011</v>
       </c>
-      <c r="D1">
+      <c r="F1">
         <v>2012</v>
       </c>
-      <c r="E1">
+      <c r="H1">
         <v>2013</v>
       </c>
-      <c r="F1">
+      <c r="J1">
         <v>2014</v>
       </c>
-      <c r="G1">
+      <c r="K1">
         <v>2015</v>
       </c>
-      <c r="H1">
+      <c r="L1">
         <v>2016</v>
       </c>
-      <c r="I1">
+      <c r="M1">
         <v>2017</v>
       </c>
-      <c r="J1">
+      <c r="N1">
         <v>2018</v>
       </c>
-      <c r="K1">
+      <c r="O1">
         <v>2019</v>
       </c>
-      <c r="L1">
+      <c r="P1">
         <v>2020</v>
       </c>
-      <c r="M1">
+      <c r="Q1">
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="14">
+        <v>0.26941300000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0.217417</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0.204462</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0.24557799999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
+      <c r="C3" s="14">
+        <v>0.18924299999999999</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="14">
+        <v>0.127891</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0.18454699999999999</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="14">
+        <v>0.16948299999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0.112663</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.111036</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.16886000000000001</v>
+      </c>
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="14">
+        <v>0.16720699999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
+      <c r="C5" s="14">
+        <v>0.10771600000000001</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="14">
+        <v>0.11074299999999999</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.151119</v>
+      </c>
+      <c r="H5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="I5" s="14">
+        <v>0.164546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="14">
+        <v>6.7022999999999999E-2</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="14">
+        <v>7.9580999999999999E-2</v>
+      </c>
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="14">
+        <v>0.118437</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.15978600000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0.15704599999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0.39664700000000003</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0.53973199999999999</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14">
+        <v>0.39655600000000002</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="14">
+        <v>0.35891600000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0.39654899999999998</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.47835699999999998</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0.37610500000000002</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0.33657999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
+      <c r="C11" s="14">
+        <v>0.25202999999999998</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="14">
+        <v>0.27761799999999998</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0.34343000000000001</v>
+      </c>
+      <c r="H11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="14">
+        <v>0.29471000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="14">
+        <v>0.169793</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="E12" s="14">
+        <v>0.24079700000000001</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0.288966</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0.28757300000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0.16755400000000001</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.23208400000000001</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="14">
+        <v>0.26922099999999999</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="14">
+        <v>0.201822</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1557,9 +1714,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated factor record with dataset 5 updated
</commit_message>
<xml_diff>
--- a/factor_record.xlsx
+++ b/factor_record.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern 1\Desktop\intern_work\Stock-market-predictor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Desktop\Stock-market-predictor-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037301E2-C1EF-4BC9-A036-DE2B08DF358B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4229E8-7D51-4975-90A6-E07B7873695F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
   <si>
     <t>Ev/EBIDTA</t>
   </si>
@@ -102,13 +102,16 @@
   </si>
   <si>
     <t>PBIDTM(%)</t>
+  </si>
+  <si>
+    <t>Total Debt/Equity(x)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +279,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="37">
@@ -643,7 +653,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -677,13 +687,14 @@
     <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1041,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1114,10 +1125,10 @@
         <v>0.24557799999999999</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="17">
-        <v>0.12884799999999999</v>
+        <v>2</v>
+      </c>
+      <c r="K2" s="15">
+        <v>0.14013900000000001</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1146,10 +1157,10 @@
         <v>0.16948299999999999</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="17">
-        <v>6.8411E-2</v>
+        <v>13</v>
+      </c>
+      <c r="K3" s="15">
+        <v>8.9484999999999995E-2</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1178,10 +1189,10 @@
         <v>0.16720699999999999</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="17">
-        <v>5.2921999999999997E-2</v>
+        <v>9</v>
+      </c>
+      <c r="K4" s="15">
+        <v>8.6527000000000007E-2</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1209,14 +1220,14 @@
       <c r="I5" s="8">
         <v>0.164546</v>
       </c>
-      <c r="J5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="17">
-        <v>3.5106999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="15">
+        <v>7.8437000000000007E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
@@ -1241,11 +1252,11 @@
       <c r="I6" s="8">
         <v>0.15978600000000001</v>
       </c>
-      <c r="J6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="17">
-        <v>3.2009000000000003E-2</v>
+      <c r="J6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="15">
+        <v>7.4213000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1290,7 +1301,7 @@
       <c r="J9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="15">
         <v>0.31676599999999999</v>
       </c>
     </row>
@@ -1322,7 +1333,7 @@
       <c r="J10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="15">
         <v>0.277223</v>
       </c>
     </row>
@@ -1354,7 +1365,7 @@
       <c r="J11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="17">
+      <c r="K11" s="15">
         <v>0.23738799999999999</v>
       </c>
     </row>
@@ -1386,7 +1397,7 @@
       <c r="J12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K12" s="15">
         <v>0.223798</v>
       </c>
     </row>
@@ -1418,7 +1429,7 @@
       <c r="J13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="15">
         <v>0.214393</v>
       </c>
     </row>
@@ -1434,26 +1445,26 @@
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1474,13 +1485,13 @@
     </row>
     <row r="20" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
       <c r="G20" s="3"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1505,13 +1516,13 @@
     </row>
     <row r="23" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>

</xml_diff>